<commit_message>
manuali oper kataster done pa nr objekti
</commit_message>
<xml_diff>
--- a/4-Te-dhenat-per-kataster/regjistri/17-Regjistri-i-ndërrimeve-për-ndertesë-Dior.xlsx
+++ b/4-Te-dhenat-per-kataster/regjistri/17-Regjistri-i-ndërrimeve-për-ndertesë-Dior.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Ferizaj\Ferizaj\Ingjinierike\565-6-Shefkia1\4-Te-dhenat-per-kataster\regjistri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Ferizaj\Sojevë\INXHINIERIKE\Dior\4-Te-dhenat-per-kataster\regjistri\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet2!$A$1:$P$26</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet2!$A$1:$P$25</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Nr</t>
   </si>
@@ -86,39 +86,15 @@
     <t>Pronari / Shfrytëzuesi                                                                      Emri (Emri i prindit) Mbiemri</t>
   </si>
   <si>
-    <t>P+4+NK</t>
-  </si>
-  <si>
     <t>Kati 1</t>
   </si>
   <si>
-    <t>Nënkulm</t>
-  </si>
-  <si>
-    <t>Rr. " Brahim Ademaj"</t>
-  </si>
-  <si>
     <t>Afarizëm/Banim</t>
   </si>
   <si>
     <t>Ferizaj</t>
   </si>
   <si>
-    <t>O-72217092-00565-6-____-___</t>
-  </si>
-  <si>
-    <t>SARAISHTE</t>
-  </si>
-  <si>
-    <t>Gjeodeti/kompania e licencuar: SEAD PRUSHI</t>
-  </si>
-  <si>
-    <t>Nr i licencës: 152</t>
-  </si>
-  <si>
-    <t>Shefki (Musli) Ugzmajli</t>
-  </si>
-  <si>
     <t>Gjithsej:</t>
   </si>
   <si>
@@ -128,7 +104,31 @@
     <t>Kati 3</t>
   </si>
   <si>
-    <t>Kati 4</t>
+    <t>B+P+3</t>
+  </si>
+  <si>
+    <t>Nr i licencës: 140</t>
+  </si>
+  <si>
+    <t>O-72217082-01997-0-____-___</t>
+  </si>
+  <si>
+    <t>Bodrumi</t>
+  </si>
+  <si>
+    <t>Shaip (Januz) Kqiku</t>
+  </si>
+  <si>
+    <t>SHAVAR</t>
+  </si>
+  <si>
+    <t>Rr. Magjistralja Ferizaj-Gjilan</t>
+  </si>
+  <si>
+    <t>Sojevë</t>
+  </si>
+  <si>
+    <t>Gjeodeti/kompania e licencuar: LIRIDON SEJDIU</t>
   </si>
 </sst>
 </file>
@@ -485,10 +485,34 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -526,30 +550,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -940,10 +940,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q672"/>
+  <dimension ref="A1:Q671"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11:O17"/>
+      <selection activeCell="D11" sqref="D11:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,170 +966,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
     </row>
     <row r="3" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="32"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="18"/>
     </row>
     <row r="10" spans="1:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1165,11 +1165,11 @@
       <c r="K10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L10" s="33" t="s">
+      <c r="L10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
       <c r="O10" s="10" t="s">
         <v>9</v>
       </c>
@@ -1178,188 +1178,173 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34">
+      <c r="A11" s="22">
         <v>1</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="12">
+        <v>330.4</v>
+      </c>
+      <c r="H11" s="20">
+        <v>408.7</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="20">
+        <v>1005022530</v>
+      </c>
+      <c r="P11" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="6"/>
+    </row>
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="11">
+        <v>411.35</v>
+      </c>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="6"/>
+    </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="11">
+        <v>399.84</v>
+      </c>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="11">
+        <v>377.81</v>
+      </c>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="6"/>
+    </row>
+    <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="12">
-        <v>208.47</v>
-      </c>
-      <c r="H11" s="14">
-        <v>208.47</v>
-      </c>
-      <c r="I11" s="14" t="s">
+      <c r="G15" s="11">
+        <v>377.81</v>
+      </c>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="6"/>
+    </row>
+    <row r="16" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="23"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="14">
-        <v>250018287</v>
-      </c>
-      <c r="P11" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q11" s="6"/>
-    </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="11">
-        <v>252.09</v>
-      </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="6"/>
-    </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="11">
-        <v>252.09</v>
-      </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="6"/>
-    </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="11">
-        <v>252.09</v>
-      </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="6"/>
-    </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="11">
-        <v>252.09</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="6"/>
-    </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="11">
-        <v>136.41</v>
-      </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="16"/>
-    </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="13">
-        <f>SUM(G11:G16)</f>
-        <v>1353.24</v>
-      </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="17"/>
+      <c r="G16" s="13">
+        <f>SUM(G11:G15)</f>
+        <v>1897.2099999999998</v>
+      </c>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="25"/>
+    </row>
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L18" s="1"/>
@@ -1368,64 +1353,58 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P19" s="5"/>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P20" s="5"/>
     </row>
-    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P21" s="5"/>
-    </row>
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24" t="s">
+    <row r="23" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="26"/>
-    </row>
-    <row r="26" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="25"/>
-      <c r="P26" s="27"/>
-    </row>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="34"/>
+    </row>
+    <row r="25" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="30"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="35"/>
+    </row>
+    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1438,16 +1417,16 @@
     <row r="36" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P39" s="5"/>
+    </row>
     <row r="40" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P40" s="5"/>
     </row>
     <row r="41" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P41" s="5"/>
     </row>
-    <row r="42" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P42" s="5"/>
-    </row>
+    <row r="42" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1463,18 +1442,18 @@
     <row r="55" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P60" s="5"/>
+    </row>
     <row r="61" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P61" s="5"/>
     </row>
     <row r="62" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P62" s="5"/>
     </row>
-    <row r="63" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P63" s="5"/>
-    </row>
+    <row r="63" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="64" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1482,16 +1461,18 @@
     <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="70" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P81" s="5"/>
+    </row>
     <row r="82" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P82" s="5"/>
     </row>
     <row r="83" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P83" s="5"/>
     </row>
-    <row r="84" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P84" s="5"/>
+    <row r="102" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P102" s="5"/>
     </row>
     <row r="103" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P103" s="5"/>
@@ -1499,8 +1480,8 @@
     <row r="104" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P104" s="5"/>
     </row>
-    <row r="105" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P105" s="5"/>
+    <row r="123" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P123" s="5"/>
     </row>
     <row r="124" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P124" s="5"/>
@@ -1508,8 +1489,8 @@
     <row r="125" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P125" s="5"/>
     </row>
-    <row r="126" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P126" s="5"/>
+    <row r="144" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P144" s="5"/>
     </row>
     <row r="145" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P145" s="5"/>
@@ -1517,8 +1498,8 @@
     <row r="146" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P146" s="5"/>
     </row>
-    <row r="147" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P147" s="5"/>
+    <row r="165" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P165" s="5"/>
     </row>
     <row r="166" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P166" s="5"/>
@@ -1526,8 +1507,8 @@
     <row r="167" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P167" s="5"/>
     </row>
-    <row r="168" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P168" s="5"/>
+    <row r="186" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P186" s="5"/>
     </row>
     <row r="187" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P187" s="5"/>
@@ -1535,8 +1516,8 @@
     <row r="188" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P188" s="5"/>
     </row>
-    <row r="189" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P189" s="5"/>
+    <row r="207" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P207" s="5"/>
     </row>
     <row r="208" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P208" s="5"/>
@@ -1544,8 +1525,8 @@
     <row r="209" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P209" s="5"/>
     </row>
-    <row r="210" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P210" s="5"/>
+    <row r="228" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P228" s="5"/>
     </row>
     <row r="229" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P229" s="5"/>
@@ -1553,8 +1534,8 @@
     <row r="230" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P230" s="5"/>
     </row>
-    <row r="231" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P231" s="5"/>
+    <row r="249" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P249" s="5"/>
     </row>
     <row r="250" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P250" s="5"/>
@@ -1562,8 +1543,8 @@
     <row r="251" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P251" s="5"/>
     </row>
-    <row r="252" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P252" s="5"/>
+    <row r="270" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P270" s="5"/>
     </row>
     <row r="271" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P271" s="5"/>
@@ -1571,8 +1552,8 @@
     <row r="272" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P272" s="5"/>
     </row>
-    <row r="273" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P273" s="5"/>
+    <row r="291" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P291" s="5"/>
     </row>
     <row r="292" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P292" s="5"/>
@@ -1580,8 +1561,8 @@
     <row r="293" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P293" s="5"/>
     </row>
-    <row r="294" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P294" s="5"/>
+    <row r="312" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P312" s="5"/>
     </row>
     <row r="313" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P313" s="5"/>
@@ -1589,8 +1570,8 @@
     <row r="314" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P314" s="5"/>
     </row>
-    <row r="315" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P315" s="5"/>
+    <row r="333" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P333" s="5"/>
     </row>
     <row r="334" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P334" s="5"/>
@@ -1598,8 +1579,8 @@
     <row r="335" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P335" s="5"/>
     </row>
-    <row r="336" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P336" s="5"/>
+    <row r="354" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P354" s="5"/>
     </row>
     <row r="355" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P355" s="5"/>
@@ -1607,8 +1588,8 @@
     <row r="356" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P356" s="5"/>
     </row>
-    <row r="357" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P357" s="5"/>
+    <row r="375" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P375" s="5"/>
     </row>
     <row r="376" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P376" s="5"/>
@@ -1616,8 +1597,8 @@
     <row r="377" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P377" s="5"/>
     </row>
-    <row r="378" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P378" s="5"/>
+    <row r="396" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P396" s="5"/>
     </row>
     <row r="397" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P397" s="5"/>
@@ -1625,8 +1606,8 @@
     <row r="398" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P398" s="5"/>
     </row>
-    <row r="399" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P399" s="5"/>
+    <row r="417" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P417" s="5"/>
     </row>
     <row r="418" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P418" s="5"/>
@@ -1634,8 +1615,8 @@
     <row r="419" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P419" s="5"/>
     </row>
-    <row r="420" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P420" s="5"/>
+    <row r="438" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P438" s="5"/>
     </row>
     <row r="439" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P439" s="5"/>
@@ -1643,8 +1624,8 @@
     <row r="440" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P440" s="5"/>
     </row>
-    <row r="441" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P441" s="5"/>
+    <row r="459" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P459" s="5"/>
     </row>
     <row r="460" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P460" s="5"/>
@@ -1652,8 +1633,8 @@
     <row r="461" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P461" s="5"/>
     </row>
-    <row r="462" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P462" s="5"/>
+    <row r="480" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P480" s="5"/>
     </row>
     <row r="481" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P481" s="5"/>
@@ -1661,8 +1642,8 @@
     <row r="482" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P482" s="5"/>
     </row>
-    <row r="483" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P483" s="5"/>
+    <row r="501" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P501" s="5"/>
     </row>
     <row r="502" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P502" s="5"/>
@@ -1670,8 +1651,8 @@
     <row r="503" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P503" s="5"/>
     </row>
-    <row r="504" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P504" s="5"/>
+    <row r="522" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P522" s="5"/>
     </row>
     <row r="523" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P523" s="5"/>
@@ -1679,8 +1660,8 @@
     <row r="524" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P524" s="5"/>
     </row>
-    <row r="525" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P525" s="5"/>
+    <row r="543" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P543" s="5"/>
     </row>
     <row r="544" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P544" s="5"/>
@@ -1688,8 +1669,8 @@
     <row r="545" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P545" s="5"/>
     </row>
-    <row r="546" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P546" s="5"/>
+    <row r="564" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P564" s="5"/>
     </row>
     <row r="565" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P565" s="5"/>
@@ -1697,8 +1678,8 @@
     <row r="566" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P566" s="5"/>
     </row>
-    <row r="567" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P567" s="5"/>
+    <row r="585" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P585" s="5"/>
     </row>
     <row r="586" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P586" s="5"/>
@@ -1706,8 +1687,8 @@
     <row r="587" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P587" s="5"/>
     </row>
-    <row r="588" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P588" s="5"/>
+    <row r="606" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P606" s="5"/>
     </row>
     <row r="607" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P607" s="5"/>
@@ -1715,8 +1696,8 @@
     <row r="608" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P608" s="5"/>
     </row>
-    <row r="609" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P609" s="5"/>
+    <row r="627" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P627" s="5"/>
     </row>
     <row r="628" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P628" s="5"/>
@@ -1724,8 +1705,8 @@
     <row r="629" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P629" s="5"/>
     </row>
-    <row r="630" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P630" s="5"/>
+    <row r="648" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P648" s="5"/>
     </row>
     <row r="649" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P649" s="5"/>
@@ -1733,8 +1714,8 @@
     <row r="650" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P650" s="5"/>
     </row>
-    <row r="651" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P651" s="5"/>
+    <row r="669" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P669" s="5"/>
     </row>
     <row r="670" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P670" s="5"/>
@@ -1742,30 +1723,27 @@
     <row r="671" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P671" s="5"/>
     </row>
-    <row r="672" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P672" s="5"/>
-    </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A24:D25"/>
+    <mergeCell ref="E24:H25"/>
+    <mergeCell ref="I24:P25"/>
     <mergeCell ref="A4:P8"/>
     <mergeCell ref="A1:P3"/>
     <mergeCell ref="A9:P9"/>
     <mergeCell ref="L10:N10"/>
-    <mergeCell ref="E11:E17"/>
-    <mergeCell ref="D11:D17"/>
-    <mergeCell ref="C11:C17"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="H11:H17"/>
-    <mergeCell ref="I11:I17"/>
-    <mergeCell ref="J11:J17"/>
-    <mergeCell ref="K11:K17"/>
-    <mergeCell ref="O11:O17"/>
-    <mergeCell ref="P11:P17"/>
-    <mergeCell ref="L11:N17"/>
-    <mergeCell ref="A25:D26"/>
-    <mergeCell ref="E25:H26"/>
-    <mergeCell ref="I25:P26"/>
+    <mergeCell ref="E11:E16"/>
+    <mergeCell ref="D11:D16"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="H11:H16"/>
+    <mergeCell ref="I11:I16"/>
+    <mergeCell ref="J11:J16"/>
+    <mergeCell ref="K11:K16"/>
+    <mergeCell ref="O11:O16"/>
+    <mergeCell ref="P11:P16"/>
+    <mergeCell ref="L11:N16"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
regjistri done pa bodrumin
</commit_message>
<xml_diff>
--- a/4-Te-dhenat-per-kataster/regjistri/17-Regjistri-i-ndërrimeve-për-ndertesë-Dior.xlsx
+++ b/4-Te-dhenat-per-kataster/regjistri/17-Regjistri-i-ndërrimeve-për-ndertesë-Dior.xlsx
@@ -110,9 +110,6 @@
     <t>Nr i licencës: 140</t>
   </si>
   <si>
-    <t>O-72217082-01997-0-____-___</t>
-  </si>
-  <si>
     <t>Bodrumi</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>Gjeodeti/kompania e licencuar: LIRIDON SEJDIU</t>
+  </si>
+  <si>
+    <t>O-72217082-01997-0-386-0</t>
   </si>
 </sst>
 </file>
@@ -485,48 +485,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -550,6 +508,48 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -943,7 +943,7 @@
   <dimension ref="A1:Q671"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D16"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,170 +966,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
     </row>
     <row r="3" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="18"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="26"/>
     </row>
     <row r="10" spans="1:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1165,11 +1165,11 @@
       <c r="K10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L10" s="19" t="s">
+      <c r="L10" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
       <c r="O10" s="10" t="s">
         <v>9</v>
       </c>
@@ -1178,150 +1178,150 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="30">
         <v>1</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="20" t="s">
+      <c r="C11" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="G11" s="12">
         <v>330.4</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="28">
         <v>408.7</v>
       </c>
-      <c r="I11" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" s="20" t="s">
+      <c r="I11" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="J11" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="20">
+      <c r="L11" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="28">
         <v>1005022530</v>
       </c>
-      <c r="P11" s="24" t="s">
+      <c r="P11" s="32" t="s">
         <v>6</v>
       </c>
       <c r="Q11" s="6"/>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G12" s="11">
         <v>411.35</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="24"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="32"/>
       <c r="Q12" s="6"/>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
       <c r="F13" s="11" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="11">
         <v>399.84</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="24"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="32"/>
       <c r="Q13" s="6"/>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
       <c r="F14" s="11" t="s">
         <v>23</v>
       </c>
       <c r="G14" s="11">
         <v>377.81</v>
       </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="24"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="32"/>
       <c r="Q14" s="6"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
       <c r="F15" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G15" s="11">
         <v>377.81</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="24"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="32"/>
       <c r="Q15" s="6"/>
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
       <c r="F16" s="13" t="s">
         <v>22</v>
       </c>
@@ -1329,15 +1329,15 @@
         <f>SUM(G11:G15)</f>
         <v>1897.2099999999998</v>
       </c>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="25"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="33"/>
     </row>
     <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L17" s="1"/>
@@ -1363,46 +1363,46 @@
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="32" t="s">
+      <c r="A24" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32" t="s">
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="34"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="20"/>
     </row>
     <row r="25" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="30"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="35"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="21"/>
     </row>
     <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1725,6 +1725,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O11:O16"/>
+    <mergeCell ref="P11:P16"/>
+    <mergeCell ref="L11:N16"/>
     <mergeCell ref="A24:D25"/>
     <mergeCell ref="E24:H25"/>
     <mergeCell ref="I24:P25"/>
@@ -1741,9 +1744,6 @@
     <mergeCell ref="I11:I16"/>
     <mergeCell ref="J11:J16"/>
     <mergeCell ref="K11:K16"/>
-    <mergeCell ref="O11:O16"/>
-    <mergeCell ref="P11:P16"/>
-    <mergeCell ref="L11:N16"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>